<commit_message>
Updated SYC to exclude pumped hydro, calibrate transp
</commit_message>
<xml_diff>
--- a/InputData/trans/SoCDTtiNTY/Share of Cargo Dist Transported that is New This Year.xlsx
+++ b/InputData/trans/SoCDTtiNTY/Share of Cargo Dist Transported that is New This Year.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code Repositories\eps-us\InputData\trans\SoCDTtiNTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Dropbox (Energy Innovation)\Documents\EPS_Models by Region\RMI\Virginia\Virginia_Model\InputData\trans\SoCDTtiNTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5060EB75-A7BB-4030-A45D-C5D5B5979CA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="21075" windowHeight="10050"/>
+    <workbookView xWindow="2445" yWindow="1140" windowWidth="10515" windowHeight="8175" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -104,7 +105,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -247,6 +248,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -282,6 +300,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -457,10 +492,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -528,13 +563,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -730,13 +767,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -804,13 +843,13 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="C3">
-        <v>3.5000000000000003E-2</v>
+        <v>0.13</v>
       </c>
       <c r="D3">
-        <v>3.5000000000000003E-2</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="E3">
-        <v>3.5000000000000003E-2</v>
+        <v>1.1299999999999999E-2</v>
       </c>
       <c r="F3">
         <v>3.5000000000000003E-2</v>

</xml_diff>

<commit_message>
Calibrate VA transp, updated cap retirements
</commit_message>
<xml_diff>
--- a/InputData/trans/SoCDTtiNTY/Share of Cargo Dist Transported that is New This Year.xlsx
+++ b/InputData/trans/SoCDTtiNTY/Share of Cargo Dist Transported that is New This Year.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-virginia\InputData\trans\SoCDTtiNTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Virginia\VA_Model\InputData\trans\SoCDTtiNTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092B58A6-BADE-46DA-912F-6024BE5CBCE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="2925" windowWidth="9930" windowHeight="13770"/>
+    <workbookView xWindow="345" yWindow="2925" windowWidth="9930" windowHeight="13770" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -104,7 +105,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -247,6 +248,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -282,6 +300,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -457,19 +492,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -477,47 +512,47 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -528,23 +563,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.1328125" customWidth="1"/>
-    <col min="2" max="8" width="14.3984375" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -570,33 +605,33 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2">
-        <v>7.8E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="C2">
-        <v>7.5499999999999998E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="D2">
-        <v>7.5499999999999998E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="E2">
-        <v>7.5499999999999998E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="F2">
-        <v>7.5499999999999998E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="G2">
-        <v>7.5499999999999998E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="H2">
-        <v>7.5499999999999998E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -622,7 +657,7 @@
         <v>4.3499999999999997E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -648,7 +683,7 @@
         <v>4.1599999999999998E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -674,7 +709,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -700,30 +735,30 @@
         <v>2.9819999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
       <c r="B7">
-        <v>5.8000000000000003E-2</v>
+        <v>5.8700000000000002E-2</v>
       </c>
       <c r="C7">
-        <v>5.8000000000000003E-2</v>
+        <v>5.8700000000000002E-2</v>
       </c>
       <c r="D7">
-        <v>5.8000000000000003E-2</v>
+        <v>5.8700000000000002E-2</v>
       </c>
       <c r="E7">
-        <v>5.8000000000000003E-2</v>
+        <v>5.8700000000000002E-2</v>
       </c>
       <c r="F7">
-        <v>5.8000000000000003E-2</v>
+        <v>5.8700000000000002E-2</v>
       </c>
       <c r="G7">
-        <v>5.8000000000000003E-2</v>
+        <v>5.8700000000000002E-2</v>
       </c>
       <c r="H7">
-        <v>5.8000000000000003E-2</v>
+        <v>5.8700000000000002E-2</v>
       </c>
     </row>
   </sheetData>
@@ -732,7 +767,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -742,13 +777,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.1328125" customWidth="1"/>
-    <col min="2" max="8" width="14.3984375" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -774,7 +809,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -800,7 +835,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -826,7 +861,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -852,7 +887,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -878,7 +913,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -904,7 +939,7 @@
         <v>3.0300000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>

</xml_diff>